<commit_message>
Results from October_30,_2020--19:05:04 run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-10-30.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-10-30.xlsx
@@ -457,25 +457,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C2" t="n">
-        <v>395458</v>
+        <v>402401</v>
       </c>
       <c r="D2" t="n">
-        <v>9675</v>
+        <v>9711</v>
       </c>
       <c r="E2" t="n">
-        <v>48114</v>
+        <v>48655</v>
       </c>
       <c r="F2" t="n">
-        <v>2326</v>
+        <v>2327</v>
       </c>
       <c r="G2" t="n">
-        <v>12.17</v>
+        <v>12.09</v>
       </c>
       <c r="H2" t="n">
-        <v>24.04</v>
+        <v>23.96</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -507,10 +507,10 @@
         <v>44125</v>
       </c>
       <c r="C3" t="n">
-        <v>181837</v>
+        <v>182270</v>
       </c>
       <c r="D3" t="n">
-        <v>5694</v>
+        <v>5705</v>
       </c>
       <c r="E3" t="n">
         <v>63549</v>
@@ -555,16 +555,16 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C4" t="n">
-        <v>105557</v>
+        <v>106573</v>
       </c>
       <c r="D4" t="n">
-        <v>2359</v>
+        <v>2366</v>
       </c>
       <c r="E4" t="n">
-        <v>4082</v>
+        <v>4104</v>
       </c>
       <c r="F4" t="n">
         <v>71</v>
@@ -573,7 +573,7 @@
         <v>5.78</v>
       </c>
       <c r="H4" t="n">
-        <v>3.05</v>
+        <v>3.04</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -582,10 +582,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>70671</v>
+        <v>70988</v>
       </c>
       <c r="L4" t="n">
-        <v>2327</v>
+        <v>2334</v>
       </c>
       <c r="M4" t="n">
         <v>269854</v>
@@ -606,25 +606,25 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C5" t="n">
-        <v>269021</v>
+        <v>271830</v>
       </c>
       <c r="D5" t="n">
-        <v>4283</v>
+        <v>4332</v>
       </c>
       <c r="E5" t="n">
-        <v>49227</v>
+        <v>49715</v>
       </c>
       <c r="F5" t="n">
-        <v>1214</v>
+        <v>1218</v>
       </c>
       <c r="G5" t="n">
-        <v>22.67</v>
+        <v>22.64</v>
       </c>
       <c r="H5" t="n">
-        <v>29.79</v>
+        <v>29.53</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -633,10 +633,10 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>217116</v>
+        <v>219550</v>
       </c>
       <c r="L5" t="n">
-        <v>4075</v>
+        <v>4124</v>
       </c>
       <c r="M5" t="n">
         <v>2179622</v>
@@ -689,13 +689,23 @@
           <t>NewYork</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="B7" s="2" t="n">
+        <v>44133</v>
+      </c>
+      <c r="C7" t="n">
+        <v>505431</v>
+      </c>
+      <c r="D7" t="n">
+        <v>25804</v>
+      </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>6474</v>
+      </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>26.64</v>
+      </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
@@ -703,12 +713,14 @@
         <v>0</v>
       </c>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>24300</v>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>An error occurred. ... TimeoutException('', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -723,12 +735,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>254091</t>
+          <t>255208</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>19336</t>
+          <t>19340</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -971,25 +983,25 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C14" t="n">
-        <v>256880</v>
+        <v>259488</v>
       </c>
       <c r="D14" t="n">
-        <v>3263</v>
+        <v>3341</v>
       </c>
       <c r="E14" t="n">
-        <v>42536</v>
+        <v>42808</v>
       </c>
       <c r="F14" t="n">
-        <v>792</v>
+        <v>798</v>
       </c>
       <c r="G14" t="n">
-        <v>16.56</v>
+        <v>16.5</v>
       </c>
       <c r="H14" t="n">
-        <v>24.27</v>
+        <v>23.89</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1051,25 +1063,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C16" t="n">
-        <v>143387</v>
+        <v>144314</v>
       </c>
       <c r="D16" t="n">
-        <v>3980</v>
+        <v>3990</v>
       </c>
       <c r="E16" t="n">
-        <v>44289</v>
+        <v>44529</v>
       </c>
       <c r="F16" t="n">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="G16" t="n">
-        <v>36.28</v>
+        <v>36.23</v>
       </c>
       <c r="H16" t="n">
-        <v>40.77</v>
+        <v>40.7</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1078,10 +1090,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>122086</v>
+        <v>122896</v>
       </c>
       <c r="L16" t="n">
-        <v>3966</v>
+        <v>3975</v>
       </c>
       <c r="M16" t="n">
         <v>1788090</v>
@@ -1102,25 +1114,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C17" t="n">
-        <v>161537</v>
+        <v>162720</v>
       </c>
       <c r="D17" t="n">
-        <v>2718</v>
+        <v>2735</v>
       </c>
       <c r="E17" t="n">
-        <v>37656</v>
+        <v>37962</v>
       </c>
       <c r="F17" t="n">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="G17" t="n">
-        <v>33.59</v>
+        <v>33.57</v>
       </c>
       <c r="H17" t="n">
-        <v>39.11</v>
+        <v>39</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1129,10 +1141,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>112110</v>
+        <v>113089</v>
       </c>
       <c r="L17" t="n">
-        <v>2636</v>
+        <v>2654</v>
       </c>
       <c r="M17" t="n">
         <v>1293186</v>
@@ -1153,25 +1165,25 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C18" t="n">
-        <v>109712</v>
+        <v>110874</v>
       </c>
       <c r="D18" t="n">
-        <v>1894</v>
+        <v>1900</v>
       </c>
       <c r="E18" t="n">
-        <v>22143</v>
+        <v>22307</v>
       </c>
       <c r="F18" t="n">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="G18" t="n">
-        <v>22.38</v>
+        <v>22.34</v>
       </c>
       <c r="H18" t="n">
-        <v>19.67</v>
+        <v>19.7</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
@@ -1180,10 +1192,10 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>98954</v>
+        <v>99869</v>
       </c>
       <c r="L18" t="n">
-        <v>1749</v>
+        <v>1756</v>
       </c>
       <c r="M18" t="n">
         <v>460970</v>
@@ -1237,25 +1249,25 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44132</v>
+        <v>44133</v>
       </c>
       <c r="C20" t="n">
-        <v>66896</v>
+        <v>67519</v>
       </c>
       <c r="D20" t="n">
-        <v>3702</v>
+        <v>3708</v>
       </c>
       <c r="E20" t="n">
-        <v>8278</v>
+        <v>8329</v>
       </c>
       <c r="F20" t="n">
         <v>674</v>
       </c>
       <c r="G20" t="n">
-        <v>12.37</v>
+        <v>12.34</v>
       </c>
       <c r="H20" t="n">
-        <v>18.21</v>
+        <v>18.18</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -1284,25 +1296,25 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C21" t="n">
-        <v>171137</v>
+        <v>174303</v>
       </c>
       <c r="D21" t="n">
-        <v>7228</v>
+        <v>7239</v>
       </c>
       <c r="E21" t="n">
-        <v>29503</v>
+        <v>29679</v>
       </c>
       <c r="F21" t="n">
-        <v>2596</v>
+        <v>2598</v>
       </c>
       <c r="G21" t="n">
-        <v>17.24</v>
+        <v>17.03</v>
       </c>
       <c r="H21" t="n">
-        <v>35.92</v>
+        <v>35.89</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -1365,26 +1377,26 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2020-10-29</t>
+          <t>2020-10-30</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>120193</v>
+        <v>121495</v>
       </c>
       <c r="D23" t="n">
-        <v>1306</v>
+        <v>1326</v>
       </c>
       <c r="E23" t="n">
-        <v>8197.1626</v>
+        <v>8273.809499999999</v>
       </c>
       <c r="F23" t="n">
-        <v>80.0578</v>
+        <v>79.95780000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>6.82</v>
+        <v>6.81</v>
       </c>
       <c r="H23" t="n">
-        <v>6.13</v>
+        <v>6.03</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
@@ -1393,10 +1405,10 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>97897.1985</v>
+        <v>98945.52800000001</v>
       </c>
       <c r="L23" t="n">
-        <v>1208.9642</v>
+        <v>1228.0086</v>
       </c>
       <c r="M23" t="n">
         <v>287959</v>
@@ -1417,16 +1429,16 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C24" t="n">
-        <v>30853</v>
+        <v>31916</v>
       </c>
       <c r="D24" t="n">
-        <v>337</v>
+        <v>364</v>
       </c>
       <c r="E24" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
@@ -1493,25 +1505,25 @@
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C26" t="n">
-        <v>11071</v>
+        <v>11314</v>
       </c>
       <c r="D26" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E26" t="n">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="F26" t="n">
         <v>3</v>
       </c>
       <c r="G26" t="n">
-        <v>4.68</v>
+        <v>4.66</v>
       </c>
       <c r="H26" t="n">
-        <v>4.11</v>
+        <v>3.9</v>
       </c>
       <c r="I26" t="b">
         <v>0</v>
@@ -1520,10 +1532,10 @@
         <v>1</v>
       </c>
       <c r="K26" t="n">
-        <v>10729</v>
+        <v>10972</v>
       </c>
       <c r="L26" t="n">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="M26" t="n">
         <v>24129</v>
@@ -1573,25 +1585,25 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C28" t="n">
-        <v>155564</v>
+        <v>157146</v>
       </c>
       <c r="D28" t="n">
-        <v>9951</v>
+        <v>9975</v>
       </c>
       <c r="E28" t="n">
-        <v>13756</v>
+        <v>13834</v>
       </c>
       <c r="F28" t="n">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="G28" t="n">
-        <v>8.84</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H28" t="n">
-        <v>7.89</v>
+        <v>7.9</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -1620,20 +1632,20 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C29" t="n">
-        <v>184669</v>
+        <v>185552</v>
       </c>
       <c r="D29" t="n">
-        <v>3634</v>
+        <v>3643</v>
       </c>
       <c r="E29" t="n">
-        <v>15937</v>
+        <v>15993</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>13.18</v>
+        <v>13.13</v>
       </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="b">
@@ -1643,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>120946</v>
+        <v>121765</v>
       </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
@@ -1665,20 +1677,20 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C30" t="n">
-        <v>45941</v>
+        <v>46424</v>
       </c>
       <c r="D30" t="n">
         <v>559</v>
       </c>
       <c r="E30" t="n">
-        <v>7291</v>
+        <v>7342</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="n">
-        <v>21.65</v>
+        <v>21.49</v>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="b">
@@ -1688,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>33680</v>
+        <v>34163</v>
       </c>
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
@@ -1713,19 +1725,19 @@
         <v>44134</v>
       </c>
       <c r="C31" t="n">
-        <v>123232</v>
+        <v>125166</v>
       </c>
       <c r="D31" t="n">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="E31" t="n">
-        <v>5688</v>
+        <v>5724</v>
       </c>
       <c r="F31" t="n">
         <v>58</v>
       </c>
       <c r="G31" t="n">
-        <v>4.62</v>
+        <v>4.57</v>
       </c>
       <c r="H31" t="n">
         <v>3.4</v>
@@ -1790,21 +1802,21 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>110640</t>
+          <t>112932</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>598</t>
+          <t>601</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1898</t>
+          <t>1928</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1816,7 +1828,7 @@
         <v>1.7</v>
       </c>
       <c r="H33" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -1995,22 +2007,22 @@
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44127</v>
+        <v>44134</v>
       </c>
       <c r="C38" t="n">
-        <v>56712</v>
+        <v>57928</v>
       </c>
       <c r="D38" t="n">
-        <v>17375</v>
+        <v>17934</v>
       </c>
       <c r="E38" t="n">
-        <v>9392</v>
+        <v>9533</v>
       </c>
       <c r="F38" t="n">
-        <v>1908</v>
+        <v>1949</v>
       </c>
       <c r="G38" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="H38" t="n">
         <v>0.11</v>
@@ -2126,19 +2138,19 @@
         </is>
       </c>
       <c r="B41" s="3" t="n">
-        <v>44132</v>
+        <v>44133</v>
       </c>
       <c r="C41" t="n">
-        <v>912904</v>
+        <v>916918</v>
       </c>
       <c r="D41" t="n">
-        <v>17541</v>
+        <v>17571</v>
       </c>
       <c r="E41" t="n">
-        <v>27247</v>
+        <v>27387</v>
       </c>
       <c r="F41" t="n">
-        <v>1292</v>
+        <v>1296</v>
       </c>
       <c r="G41" t="n">
         <v>4.21</v>
@@ -2153,10 +2165,10 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>646485</v>
+        <v>650369</v>
       </c>
       <c r="L41" t="n">
-        <v>17350</v>
+        <v>17393</v>
       </c>
       <c r="M41" t="n">
         <v>2267875</v>
@@ -2206,10 +2218,10 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C43" t="n">
-        <v>2141</v>
+        <v>2155</v>
       </c>
       <c r="D43" t="n">
         <v>58</v>
@@ -2221,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>9.91</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -2233,7 +2245,7 @@
         <v>1</v>
       </c>
       <c r="K43" t="n">
-        <v>2048</v>
+        <v>2059</v>
       </c>
       <c r="L43" t="n">
         <v>58</v>
@@ -2257,20 +2269,20 @@
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C44" t="n">
-        <v>44904</v>
+        <v>45909</v>
       </c>
       <c r="D44" t="n">
-        <v>994</v>
+        <v>1007</v>
       </c>
       <c r="E44" t="n">
-        <v>732</v>
+        <v>765</v>
       </c>
       <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
-        <v>1.63</v>
+        <v>1.67</v>
       </c>
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="b">
@@ -2300,25 +2312,25 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C45" t="n">
-        <v>784331</v>
+        <v>789714</v>
       </c>
       <c r="D45" t="n">
-        <v>16648</v>
+        <v>16720</v>
       </c>
       <c r="E45" t="n">
-        <v>103226</v>
+        <v>103732</v>
       </c>
       <c r="F45" t="n">
-        <v>2886</v>
+        <v>2893</v>
       </c>
       <c r="G45" t="n">
-        <v>13.16</v>
+        <v>13.14</v>
       </c>
       <c r="H45" t="n">
-        <v>17.34</v>
+        <v>17.3</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
@@ -2347,25 +2359,25 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C46" t="n">
-        <v>17074</v>
+        <v>17144</v>
       </c>
       <c r="D46" t="n">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E46" t="n">
-        <v>8446</v>
+        <v>8479</v>
       </c>
       <c r="F46" t="n">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G46" t="n">
-        <v>49.47</v>
+        <v>49.46</v>
       </c>
       <c r="H46" t="n">
-        <v>74.88</v>
+        <v>74.92</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -2423,25 +2435,25 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C48" t="n">
-        <v>102014</v>
+        <v>104426</v>
       </c>
       <c r="D48" t="n">
-        <v>2268</v>
+        <v>2278</v>
       </c>
       <c r="E48" t="n">
-        <v>3652</v>
+        <v>3676</v>
       </c>
       <c r="F48" t="n">
         <v>135</v>
       </c>
       <c r="G48" t="n">
-        <v>4.32</v>
+        <v>4.29</v>
       </c>
       <c r="H48" t="n">
-        <v>6.07</v>
+        <v>6.05</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2450,10 +2462,10 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>84549</v>
+        <v>85765</v>
       </c>
       <c r="L48" t="n">
-        <v>2223</v>
+        <v>2231</v>
       </c>
       <c r="M48" t="n">
         <v>227938</v>
@@ -2474,16 +2486,16 @@
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C49" t="n">
-        <v>55898</v>
+        <v>56369</v>
       </c>
       <c r="D49" t="n">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="E49" t="n">
-        <v>1972</v>
+        <v>1987</v>
       </c>
       <c r="F49" t="n">
         <v>36</v>
@@ -2492,7 +2504,7 @@
         <v>4.25</v>
       </c>
       <c r="H49" t="n">
-        <v>4.08</v>
+        <v>4.07</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
@@ -2501,10 +2513,10 @@
         <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>46398</v>
+        <v>46790</v>
       </c>
       <c r="L49" t="n">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="M49" t="n">
         <v>166412</v>
@@ -2591,16 +2603,16 @@
         </is>
       </c>
       <c r="B52" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C52" t="n">
-        <v>242480</v>
+        <v>244045</v>
       </c>
       <c r="D52" t="n">
-        <v>5918</v>
+        <v>5934</v>
       </c>
       <c r="E52" t="n">
-        <v>7461</v>
+        <v>7497</v>
       </c>
       <c r="F52" t="n">
         <v>184</v>
@@ -2609,7 +2621,7 @@
         <v>4.37</v>
       </c>
       <c r="H52" t="n">
-        <v>3.49</v>
+        <v>3.48</v>
       </c>
       <c r="I52" t="b">
         <v>0</v>
@@ -2618,10 +2630,10 @@
         <v>0</v>
       </c>
       <c r="K52" t="n">
-        <v>170671</v>
+        <v>171678</v>
       </c>
       <c r="L52" t="n">
-        <v>5278</v>
+        <v>5289</v>
       </c>
       <c r="M52" t="n">
         <v>305259</v>
@@ -2675,22 +2687,22 @@
         </is>
       </c>
       <c r="B54" s="3" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C54" t="n">
-        <v>178158</v>
+        <v>179612</v>
       </c>
       <c r="D54" t="n">
-        <v>3636</v>
+        <v>3643</v>
       </c>
       <c r="E54" t="n">
-        <v>34901</v>
+        <v>35107</v>
       </c>
       <c r="F54" t="n">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="G54" t="n">
-        <v>19.59</v>
+        <v>19.55</v>
       </c>
       <c r="H54" t="n">
         <v>26.68</v>
@@ -2751,25 +2763,25 @@
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C56" t="n">
-        <v>172730</v>
+        <v>175893</v>
       </c>
       <c r="D56" t="n">
-        <v>4024</v>
+        <v>4050</v>
       </c>
       <c r="E56" t="n">
-        <v>14280</v>
+        <v>14398</v>
       </c>
       <c r="F56" t="n">
         <v>477</v>
       </c>
       <c r="G56" t="n">
-        <v>8.27</v>
+        <v>8.19</v>
       </c>
       <c r="H56" t="n">
-        <v>11.85</v>
+        <v>11.78</v>
       </c>
       <c r="I56" t="b">
         <v>1</v>
@@ -2798,22 +2810,22 @@
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C57" t="n">
-        <v>10768</v>
+        <v>10884</v>
       </c>
       <c r="D57" t="n">
         <v>482</v>
       </c>
       <c r="E57" t="n">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="F57" t="n">
         <v>9</v>
       </c>
       <c r="G57" t="n">
-        <v>4.46</v>
+        <v>4.43</v>
       </c>
       <c r="H57" t="n">
         <v>1.97</v>
@@ -2825,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="K57" t="n">
-        <v>9291</v>
+        <v>9393</v>
       </c>
       <c r="L57" t="n">
         <v>456</v>
@@ -2849,25 +2861,25 @@
         </is>
       </c>
       <c r="B58" s="2" t="n">
-        <v>44133</v>
+        <v>44134</v>
       </c>
       <c r="C58" t="n">
-        <v>103305</v>
+        <v>105242</v>
       </c>
       <c r="D58" t="n">
-        <v>1461</v>
+        <v>1476</v>
       </c>
       <c r="E58" t="n">
-        <v>8949</v>
+        <v>9029</v>
       </c>
       <c r="F58" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G58" t="n">
-        <v>11.06</v>
+        <v>11.01</v>
       </c>
       <c r="H58" t="n">
-        <v>11.91</v>
+        <v>11.86</v>
       </c>
       <c r="I58" t="b">
         <v>0</v>
@@ -2876,10 +2888,10 @@
         <v>1</v>
       </c>
       <c r="K58" t="n">
-        <v>80918</v>
+        <v>82015</v>
       </c>
       <c r="L58" t="n">
-        <v>1360</v>
+        <v>1374</v>
       </c>
       <c r="M58" t="n">
         <v>354112</v>
@@ -2900,25 +2912,25 @@
         </is>
       </c>
       <c r="B59" s="2" t="n">
-        <v>44132</v>
+        <v>44133</v>
       </c>
       <c r="C59" t="n">
-        <v>305070</v>
+        <v>306327</v>
       </c>
       <c r="D59" t="n">
-        <v>7044</v>
+        <v>7056</v>
       </c>
       <c r="E59" t="n">
-        <v>8837</v>
+        <v>8886</v>
       </c>
       <c r="F59" t="n">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G59" t="n">
-        <v>4.79</v>
+        <v>4.78</v>
       </c>
       <c r="H59" t="n">
-        <v>9.59</v>
+        <v>9.58</v>
       </c>
       <c r="I59" t="b">
         <v>0</v>
@@ -2927,10 +2939,10 @@
         <v>0</v>
       </c>
       <c r="K59" t="n">
-        <v>184631</v>
+        <v>185731</v>
       </c>
       <c r="L59" t="n">
-        <v>6635</v>
+        <v>6649</v>
       </c>
       <c r="M59" t="n">
         <v>823987</v>

</xml_diff>